<commit_message>
added project name entry
</commit_message>
<xml_diff>
--- a/investments.xlsx
+++ b/investments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,6 +469,11 @@
           <t>Principal + Interest</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Project Name</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
resize window, add alert
</commit_message>
<xml_diff>
--- a/investments.xlsx
+++ b/investments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,42 +475,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Peter</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Mora</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2024-12-14</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2025-09-10</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>100000</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="G2" t="n">
-        <v>106000</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Long Beach Square</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added maturity date slider
</commit_message>
<xml_diff>
--- a/investments.xlsx
+++ b/investments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,6 +474,11 @@
           <t>Project Name</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Months To Maturity</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fixed add/update window buttons
</commit_message>
<xml_diff>
--- a/investments.xlsx
+++ b/investments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,6 +479,11 @@
           <t>Principal + Interest</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Auto Rollover</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>